<commit_message>
add extra IgG1 custom trait
</commit_message>
<xml_diff>
--- a/inst/extdata/Custom_traits_formulas_example.xlsx
+++ b/inst/extdata/Custom_traits_formulas_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vf-lumc-home.lumcnet.prod.intern\lumc-home$\sgijze\MyDocs\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A74850-FC65-4A52-BACE-891DA443C320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AB5E23-B83C-4873-BA55-9EB18123DEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22714" yWindow="-231" windowWidth="23040" windowHeight="13897" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>IgGI</t>
   </si>
@@ -39,10 +39,13 @@
     <t>first_trait = 0.5 * H4N4 + H5N4</t>
   </si>
   <si>
-    <t>second_trait = (H4N4F1 + H5N4F1) / H3N4F1</t>
-  </si>
-  <si>
-    <t>third_trait = H5N4F1S2 * H4N4F1S1</t>
+    <t>second_trait = H4N4 + H5N4</t>
+  </si>
+  <si>
+    <t>third_trait = (H4N4F1 + H5N4F1) / H3N4F1</t>
+  </si>
+  <si>
+    <t>fourth_trait = H5N4F1S2 * H4N4F1S1</t>
   </si>
 </sst>
 </file>
@@ -360,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -381,7 +384,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -389,10 +392,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>